<commit_message>
Minor changes to include faux septic system inputs.
</commit_message>
<xml_diff>
--- a/maui/std_input/Landuse_lookup_maui.xlsx
+++ b/maui/std_input/Landuse_lookup_maui.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smwesten/SMWData/Source_Code/swb2_examples/maui/std_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smwesten/SMWData/Static/Source_Code/swb2_examples/maui/std_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="LU_lookup_Engott_v3_6.txt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="119">
   <si>
     <t>LU code</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Depletion_fraction</t>
   </si>
   <si>
-    <t>Annual_direct_recharge_rate</t>
-  </si>
-  <si>
     <t>Kcb_Jan</t>
   </si>
   <si>
@@ -378,12 +375,21 @@
   </si>
   <si>
     <t>Max net infil 4</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Annual_direct_net_infiltration</t>
+  </si>
+  <si>
+    <t>Annual_esptic_discharge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd"/>
   </numFmts>
@@ -454,13 +460,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -816,27 +823,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BX33"/>
+  <dimension ref="A1:BY33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="AJ12" sqref="AJ12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.1640625" customWidth="1"/>
     <col min="27" max="27" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="32.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="23.33203125" customWidth="1"/>
-    <col min="52" max="52" width="13.6640625" style="1" customWidth="1"/>
-    <col min="53" max="53" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="73" max="76" width="11" style="1"/>
+    <col min="34" max="34" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.6640625" style="1" customWidth="1"/>
+    <col min="54" max="54" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="74" max="77" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -862,16 +870,16 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
         <v>113</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>114</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>115</v>
-      </c>
-      <c r="L1" t="s">
-        <v>116</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -922,7 +930,7 @@
         <v>23</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AD1" t="s">
         <v>24</v>
@@ -937,144 +945,147 @@
         <v>27</v>
       </c>
       <c r="AH1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK1" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>35</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>36</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>38</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>40</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AZ1" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BA1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="BB1" t="s">
         <v>44</v>
       </c>
-      <c r="AZ1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="BA1" t="s">
+      <c r="BC1" t="s">
         <v>45</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BD1" t="s">
         <v>46</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BE1" t="s">
         <v>47</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BF1" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG1" t="s">
         <v>48</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
+        <v>49</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BL1" t="s">
         <v>107</v>
       </c>
-      <c r="BF1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BJ1" t="s">
+      <c r="BM1" t="s">
         <v>53</v>
       </c>
-      <c r="BK1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BL1" t="s">
+      <c r="BN1" t="s">
         <v>54</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BO1" t="s">
         <v>55</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BP1" t="s">
         <v>56</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BQ1" t="s">
         <v>57</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BR1" t="s">
         <v>58</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BS1" t="s">
         <v>59</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BT1" t="s">
         <v>60</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BU1" t="s">
         <v>61</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>64</v>
       </c>
-      <c r="BW1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="BX1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1139,11 +1150,14 @@
       <c r="Z2">
         <v>0</v>
       </c>
+      <c r="AA2" t="s">
+        <v>88</v>
+      </c>
       <c r="AB2">
         <v>0</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -1164,7 +1178,7 @@
         <v>0</v>
       </c>
       <c r="AJ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK2">
         <v>1</v>
@@ -1200,7 +1214,7 @@
         <v>1</v>
       </c>
       <c r="AV2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW2">
         <v>0</v>
@@ -1211,24 +1225,24 @@
       <c r="AY2">
         <v>0</v>
       </c>
-      <c r="AZ2" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA2">
-        <v>0</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC2">
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB2">
+        <v>0</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD2">
         <v>50</v>
       </c>
-      <c r="BD2">
+      <c r="BE2">
         <v>86</v>
       </c>
-      <c r="BE2">
-        <v>0</v>
-      </c>
       <c r="BF2">
         <v>0</v>
       </c>
@@ -1272,30 +1286,33 @@
         <v>0</v>
       </c>
       <c r="BT2">
-        <v>1</v>
-      </c>
-      <c r="BU2" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU2">
+        <v>1</v>
       </c>
       <c r="BV2" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW2" s="1">
         <v>40907</v>
       </c>
-      <c r="BW2" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX2" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY2" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="3" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -1343,7 +1360,7 @@
         <v>1.5</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U3" s="2">
         <v>1.5</v>
@@ -1364,13 +1381,13 @@
         <v>6</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB3" s="2">
         <v>0</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AD3" s="2">
         <v>0</v>
@@ -1391,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="AJ3" s="2">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="AK3" s="2">
         <v>0.3</v>
@@ -1427,7 +1444,7 @@
         <v>0.3</v>
       </c>
       <c r="AV3" s="2">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AW3" s="2">
         <v>0</v>
@@ -1438,24 +1455,24 @@
       <c r="AY3" s="2">
         <v>0</v>
       </c>
-      <c r="AZ3" s="3">
-        <v>40543</v>
-      </c>
-      <c r="BA3" s="2">
+      <c r="AZ3" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BB3" s="2">
         <v>5</v>
       </c>
-      <c r="BB3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC3" s="2">
+      <c r="BC3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD3" s="2">
         <v>50</v>
       </c>
-      <c r="BD3" s="2">
+      <c r="BE3" s="2">
         <v>86</v>
       </c>
-      <c r="BE3" s="2">
-        <v>0</v>
-      </c>
       <c r="BF3" s="2">
         <v>0</v>
       </c>
@@ -1499,30 +1516,33 @@
         <v>0</v>
       </c>
       <c r="BT3" s="2">
-        <v>1</v>
-      </c>
-      <c r="BU3" s="3">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU3" s="2">
+        <v>1</v>
       </c>
       <c r="BV3" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BW3" s="3">
         <v>40907</v>
       </c>
-      <c r="BW3" s="3">
-        <v>40543</v>
-      </c>
       <c r="BX3" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BY3" s="3">
         <v>40907</v>
       </c>
     </row>
-    <row r="4" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -1588,13 +1608,13 @@
         <v>8</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB4" s="2">
         <v>0</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD4" s="2">
         <v>0</v>
@@ -1615,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="AJ4" s="2">
-        <v>0.91</v>
+        <v>0</v>
       </c>
       <c r="AK4" s="2">
         <v>0.91</v>
@@ -1651,7 +1671,7 @@
         <v>0.91</v>
       </c>
       <c r="AV4" s="2">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="AW4" s="2">
         <v>0</v>
@@ -1662,24 +1682,24 @@
       <c r="AY4" s="2">
         <v>0</v>
       </c>
-      <c r="AZ4" s="3">
-        <v>40543</v>
-      </c>
-      <c r="BA4" s="2">
+      <c r="AZ4" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA4" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BB4" s="2">
         <v>5</v>
       </c>
-      <c r="BB4" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC4" s="2">
+      <c r="BC4" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD4" s="2">
         <v>50</v>
       </c>
-      <c r="BD4" s="2">
+      <c r="BE4" s="2">
         <v>86</v>
       </c>
-      <c r="BE4" s="2">
-        <v>0</v>
-      </c>
       <c r="BF4" s="2">
         <v>0</v>
       </c>
@@ -1723,30 +1743,33 @@
         <v>0</v>
       </c>
       <c r="BT4" s="2">
-        <v>1</v>
-      </c>
-      <c r="BU4" s="3">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU4" s="2">
+        <v>1</v>
       </c>
       <c r="BV4" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BW4" s="3">
         <v>40907</v>
       </c>
-      <c r="BW4" s="3">
-        <v>40543</v>
-      </c>
       <c r="BX4" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BY4" s="3">
         <v>40907</v>
       </c>
     </row>
-    <row r="5" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -1812,13 +1835,13 @@
         <v>10</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB5" s="2">
         <v>0</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD5" s="2">
         <v>0</v>
@@ -1839,7 +1862,7 @@
         <v>0</v>
       </c>
       <c r="AJ5" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK5" s="2">
         <v>1</v>
@@ -1875,7 +1898,7 @@
         <v>1</v>
       </c>
       <c r="AV5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW5" s="2">
         <v>0</v>
@@ -1886,24 +1909,24 @@
       <c r="AY5" s="2">
         <v>0</v>
       </c>
-      <c r="AZ5" s="3">
-        <v>40543</v>
-      </c>
-      <c r="BA5" s="2">
+      <c r="AZ5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BB5" s="2">
         <v>4</v>
       </c>
-      <c r="BB5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC5" s="2">
+      <c r="BC5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD5" s="2">
         <v>50</v>
       </c>
-      <c r="BD5" s="2">
+      <c r="BE5" s="2">
         <v>86</v>
       </c>
-      <c r="BE5" s="2">
-        <v>0</v>
-      </c>
       <c r="BF5" s="2">
         <v>0</v>
       </c>
@@ -1947,30 +1970,33 @@
         <v>0</v>
       </c>
       <c r="BT5" s="2">
-        <v>1</v>
-      </c>
-      <c r="BU5" s="3">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU5" s="2">
+        <v>1</v>
       </c>
       <c r="BV5" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BW5" s="3">
         <v>40907</v>
       </c>
-      <c r="BW5" s="3">
-        <v>40543</v>
-      </c>
       <c r="BX5" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BY5" s="3">
         <v>40907</v>
       </c>
     </row>
-    <row r="6" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -2035,11 +2061,14 @@
       <c r="Z6">
         <v>0</v>
       </c>
+      <c r="AA6" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB6">
         <v>0</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -2059,8 +2088,8 @@
       <c r="AI6" s="2">
         <v>0</v>
       </c>
-      <c r="AJ6">
-        <v>0.91</v>
+      <c r="AJ6" s="2">
+        <v>0</v>
       </c>
       <c r="AK6">
         <v>0.91</v>
@@ -2096,7 +2125,7 @@
         <v>0.91</v>
       </c>
       <c r="AV6">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="AW6">
         <v>0</v>
@@ -2107,25 +2136,25 @@
       <c r="AY6">
         <v>0</v>
       </c>
-      <c r="AZ6" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA6">
+      <c r="AZ6">
+        <v>0</v>
+      </c>
+      <c r="BA6" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB6">
         <v>10</v>
       </c>
-      <c r="BB6" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC6">
+      <c r="BC6" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD6">
         <v>50</v>
       </c>
-      <c r="BD6">
+      <c r="BE6">
         <v>86</v>
       </c>
-      <c r="BE6" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF6">
+      <c r="BF6" s="2">
         <v>0</v>
       </c>
       <c r="BG6">
@@ -2140,10 +2169,10 @@
       <c r="BJ6">
         <v>0</v>
       </c>
-      <c r="BK6" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL6">
+      <c r="BK6">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="2">
         <v>0</v>
       </c>
       <c r="BM6">
@@ -2168,30 +2197,33 @@
         <v>0</v>
       </c>
       <c r="BT6">
-        <v>1</v>
-      </c>
-      <c r="BU6" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU6">
+        <v>1</v>
       </c>
       <c r="BV6" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW6" s="1">
         <v>40907</v>
       </c>
-      <c r="BW6" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX6" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY6" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -2256,11 +2288,14 @@
       <c r="Z7">
         <v>0</v>
       </c>
+      <c r="AA7" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB7">
         <v>0</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -2280,8 +2315,8 @@
       <c r="AI7" s="2">
         <v>0</v>
       </c>
-      <c r="AJ7">
-        <v>0.95</v>
+      <c r="AJ7" s="2">
+        <v>0</v>
       </c>
       <c r="AK7">
         <v>0.95</v>
@@ -2317,7 +2352,7 @@
         <v>0.95</v>
       </c>
       <c r="AV7">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AW7">
         <v>0</v>
@@ -2328,25 +2363,25 @@
       <c r="AY7">
         <v>0</v>
       </c>
-      <c r="AZ7" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA7">
+      <c r="AZ7">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB7">
         <v>3</v>
       </c>
-      <c r="BB7" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC7">
+      <c r="BC7" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD7">
         <v>50</v>
       </c>
-      <c r="BD7">
+      <c r="BE7">
         <v>86</v>
       </c>
-      <c r="BE7" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF7">
+      <c r="BF7" s="2">
         <v>0</v>
       </c>
       <c r="BG7">
@@ -2361,10 +2396,10 @@
       <c r="BJ7">
         <v>0</v>
       </c>
-      <c r="BK7" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL7">
+      <c r="BK7">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="2">
         <v>0</v>
       </c>
       <c r="BM7">
@@ -2389,30 +2424,33 @@
         <v>0</v>
       </c>
       <c r="BT7">
-        <v>1</v>
-      </c>
-      <c r="BU7" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU7">
+        <v>1</v>
       </c>
       <c r="BV7" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW7" s="1">
         <v>40907</v>
       </c>
-      <c r="BW7" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX7" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY7" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -2477,11 +2515,14 @@
       <c r="Z8">
         <v>0</v>
       </c>
+      <c r="AA8" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB8">
         <v>0</v>
       </c>
       <c r="AC8" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -2501,8 +2542,8 @@
       <c r="AI8" s="2">
         <v>0</v>
       </c>
-      <c r="AJ8">
-        <v>1.18</v>
+      <c r="AJ8" s="2">
+        <v>0</v>
       </c>
       <c r="AK8">
         <v>1.18</v>
@@ -2538,7 +2579,7 @@
         <v>1.18</v>
       </c>
       <c r="AV8">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="AW8">
         <v>0</v>
@@ -2549,25 +2590,25 @@
       <c r="AY8">
         <v>0</v>
       </c>
-      <c r="AZ8" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA8">
+      <c r="AZ8">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB8">
         <v>2</v>
       </c>
-      <c r="BB8" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC8">
+      <c r="BC8" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD8">
         <v>50</v>
       </c>
-      <c r="BD8">
+      <c r="BE8">
         <v>86</v>
       </c>
-      <c r="BE8" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF8">
+      <c r="BF8" s="2">
         <v>0</v>
       </c>
       <c r="BG8">
@@ -2582,10 +2623,10 @@
       <c r="BJ8">
         <v>0</v>
       </c>
-      <c r="BK8" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL8">
+      <c r="BK8">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="2">
         <v>0</v>
       </c>
       <c r="BM8">
@@ -2610,27 +2651,30 @@
         <v>0</v>
       </c>
       <c r="BT8">
-        <v>1</v>
-      </c>
-      <c r="BU8" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU8">
+        <v>1</v>
       </c>
       <c r="BV8" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW8" s="1">
         <v>40907</v>
       </c>
-      <c r="BW8" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX8" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY8" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <v>18</v>
@@ -2698,11 +2742,14 @@
       <c r="Z9">
         <v>0</v>
       </c>
+      <c r="AA9" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB9">
         <v>0</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD9">
         <v>0</v>
@@ -2722,8 +2769,8 @@
       <c r="AI9" s="2">
         <v>0</v>
       </c>
-      <c r="AJ9">
-        <v>1.18</v>
+      <c r="AJ9" s="2">
+        <v>0</v>
       </c>
       <c r="AK9">
         <v>1.18</v>
@@ -2759,7 +2806,7 @@
         <v>1.18</v>
       </c>
       <c r="AV9">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="AW9">
         <v>0</v>
@@ -2770,25 +2817,25 @@
       <c r="AY9">
         <v>0</v>
       </c>
-      <c r="AZ9" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA9">
+      <c r="AZ9">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB9">
         <v>2</v>
       </c>
-      <c r="BB9" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC9">
+      <c r="BC9" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD9">
         <v>50</v>
       </c>
-      <c r="BD9">
+      <c r="BE9">
         <v>86</v>
       </c>
-      <c r="BE9" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF9">
+      <c r="BF9" s="2">
         <v>0</v>
       </c>
       <c r="BG9">
@@ -2803,10 +2850,10 @@
       <c r="BJ9">
         <v>0</v>
       </c>
-      <c r="BK9" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL9">
+      <c r="BK9">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="2">
         <v>0</v>
       </c>
       <c r="BM9">
@@ -2831,27 +2878,30 @@
         <v>0</v>
       </c>
       <c r="BT9">
-        <v>1</v>
-      </c>
-      <c r="BU9" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU9">
+        <v>1</v>
       </c>
       <c r="BV9" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW9" s="1">
         <v>40907</v>
       </c>
-      <c r="BW9" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX9" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY9" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="10" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2">
         <v>58</v>
@@ -2920,13 +2970,13 @@
         <v>1</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB10" s="2">
         <v>0</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD10" s="2">
         <v>0</v>
@@ -2947,7 +2997,7 @@
         <v>1</v>
       </c>
       <c r="AJ10" s="2">
-        <v>1.18</v>
+        <v>6</v>
       </c>
       <c r="AK10" s="2">
         <v>1.18</v>
@@ -2983,7 +3033,7 @@
         <v>1.18</v>
       </c>
       <c r="AV10" s="2">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="AW10" s="2">
         <v>0</v>
@@ -2994,24 +3044,24 @@
       <c r="AY10" s="2">
         <v>0</v>
       </c>
-      <c r="AZ10" s="3">
-        <v>40543</v>
-      </c>
-      <c r="BA10" s="2">
+      <c r="AZ10" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BB10" s="2">
         <v>2</v>
       </c>
-      <c r="BB10" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC10" s="2">
+      <c r="BC10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD10" s="2">
         <v>50</v>
       </c>
-      <c r="BD10" s="2">
+      <c r="BE10" s="2">
         <v>86</v>
       </c>
-      <c r="BE10" s="2">
-        <v>0</v>
-      </c>
       <c r="BF10" s="2">
         <v>0</v>
       </c>
@@ -3055,27 +3105,30 @@
         <v>0</v>
       </c>
       <c r="BT10" s="2">
-        <v>1</v>
-      </c>
-      <c r="BU10" s="3">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU10" s="2">
+        <v>1</v>
       </c>
       <c r="BV10" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BW10" s="3">
         <v>40907</v>
       </c>
-      <c r="BW10" s="3">
-        <v>40543</v>
-      </c>
       <c r="BX10" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BY10" s="3">
         <v>40907</v>
       </c>
     </row>
-    <row r="11" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2">
         <v>84</v>
@@ -3144,13 +3197,13 @@
         <v>1</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB11" s="2">
         <v>0</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD11" s="2">
         <v>0</v>
@@ -3171,7 +3224,7 @@
         <v>1</v>
       </c>
       <c r="AJ11" s="2">
-        <v>1.18</v>
+        <v>6</v>
       </c>
       <c r="AK11" s="2">
         <v>1.18</v>
@@ -3207,7 +3260,7 @@
         <v>1.18</v>
       </c>
       <c r="AV11" s="2">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="AW11" s="2">
         <v>0</v>
@@ -3218,24 +3271,24 @@
       <c r="AY11" s="2">
         <v>0</v>
       </c>
-      <c r="AZ11" s="3">
-        <v>40543</v>
-      </c>
-      <c r="BA11" s="2">
+      <c r="AZ11" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA11" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BB11" s="2">
         <v>2</v>
       </c>
-      <c r="BB11" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC11" s="2">
+      <c r="BC11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD11" s="2">
         <v>50</v>
       </c>
-      <c r="BD11" s="2">
+      <c r="BE11" s="2">
         <v>86</v>
       </c>
-      <c r="BE11" s="2">
-        <v>0</v>
-      </c>
       <c r="BF11" s="2">
         <v>0</v>
       </c>
@@ -3279,30 +3332,33 @@
         <v>0</v>
       </c>
       <c r="BT11" s="2">
-        <v>1</v>
-      </c>
-      <c r="BU11" s="3">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU11" s="2">
+        <v>1</v>
       </c>
       <c r="BV11" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BW11" s="3">
         <v>40907</v>
       </c>
-      <c r="BW11" s="3">
-        <v>40543</v>
-      </c>
       <c r="BX11" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BY11" s="3">
         <v>40907</v>
       </c>
     </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -3367,11 +3423,14 @@
       <c r="Z12">
         <v>0</v>
       </c>
+      <c r="AA12" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB12">
         <v>0</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD12">
         <v>0</v>
@@ -3391,8 +3450,8 @@
       <c r="AI12" s="2">
         <v>0</v>
       </c>
-      <c r="AJ12">
-        <v>1.05</v>
+      <c r="AJ12" s="2">
+        <v>0</v>
       </c>
       <c r="AK12">
         <v>1.05</v>
@@ -3428,7 +3487,7 @@
         <v>1.05</v>
       </c>
       <c r="AV12">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="AW12">
         <v>0</v>
@@ -3439,25 +3498,25 @@
       <c r="AY12">
         <v>0</v>
       </c>
-      <c r="AZ12" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA12">
-        <v>0</v>
-      </c>
-      <c r="BB12" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC12">
+      <c r="AZ12">
+        <v>0</v>
+      </c>
+      <c r="BA12" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB12">
+        <v>0</v>
+      </c>
+      <c r="BC12" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD12">
         <v>50</v>
       </c>
-      <c r="BD12">
+      <c r="BE12">
         <v>86</v>
       </c>
-      <c r="BE12" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF12">
+      <c r="BF12" s="2">
         <v>0</v>
       </c>
       <c r="BG12">
@@ -3472,10 +3531,10 @@
       <c r="BJ12">
         <v>0</v>
       </c>
-      <c r="BK12" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL12">
+      <c r="BK12">
+        <v>0</v>
+      </c>
+      <c r="BL12" s="2">
         <v>0</v>
       </c>
       <c r="BM12">
@@ -3500,30 +3559,33 @@
         <v>0</v>
       </c>
       <c r="BT12">
-        <v>1</v>
-      </c>
-      <c r="BU12" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU12">
+        <v>1</v>
       </c>
       <c r="BV12" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW12" s="1">
         <v>40907</v>
       </c>
-      <c r="BW12" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX12" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY12" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="13" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -3588,11 +3650,14 @@
       <c r="Z13">
         <v>0</v>
       </c>
+      <c r="AA13" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB13">
         <v>0</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD13">
         <v>0</v>
@@ -3612,8 +3677,8 @@
       <c r="AI13" s="2">
         <v>0</v>
       </c>
-      <c r="AJ13">
-        <v>1.18</v>
+      <c r="AJ13" s="2">
+        <v>0</v>
       </c>
       <c r="AK13">
         <v>1.18</v>
@@ -3649,7 +3714,7 @@
         <v>1.18</v>
       </c>
       <c r="AV13">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="AW13">
         <v>0</v>
@@ -3660,25 +3725,25 @@
       <c r="AY13">
         <v>0</v>
       </c>
-      <c r="AZ13" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA13">
+      <c r="AZ13">
+        <v>0</v>
+      </c>
+      <c r="BA13" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB13">
         <v>3</v>
       </c>
-      <c r="BB13" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC13">
+      <c r="BC13" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD13">
         <v>50</v>
       </c>
-      <c r="BD13">
+      <c r="BE13">
         <v>86</v>
       </c>
-      <c r="BE13" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF13">
+      <c r="BF13" s="2">
         <v>0</v>
       </c>
       <c r="BG13">
@@ -3693,10 +3758,10 @@
       <c r="BJ13">
         <v>0</v>
       </c>
-      <c r="BK13" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL13">
+      <c r="BK13">
+        <v>0</v>
+      </c>
+      <c r="BL13" s="2">
         <v>0</v>
       </c>
       <c r="BM13">
@@ -3721,30 +3786,33 @@
         <v>0</v>
       </c>
       <c r="BT13">
-        <v>1</v>
-      </c>
-      <c r="BU13" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU13">
+        <v>1</v>
       </c>
       <c r="BV13" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW13" s="1">
         <v>40907</v>
       </c>
-      <c r="BW13" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX13" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY13" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -3809,11 +3877,14 @@
       <c r="Z14">
         <v>0</v>
       </c>
+      <c r="AA14" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB14">
         <v>0</v>
       </c>
       <c r="AC14" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -3833,8 +3904,8 @@
       <c r="AI14" s="2">
         <v>0</v>
       </c>
-      <c r="AJ14">
-        <v>1.18</v>
+      <c r="AJ14" s="2">
+        <v>0</v>
       </c>
       <c r="AK14">
         <v>1.18</v>
@@ -3870,7 +3941,7 @@
         <v>1.18</v>
       </c>
       <c r="AV14">
-        <v>0</v>
+        <v>1.18</v>
       </c>
       <c r="AW14">
         <v>0</v>
@@ -3881,25 +3952,25 @@
       <c r="AY14">
         <v>0</v>
       </c>
-      <c r="AZ14" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA14">
+      <c r="AZ14">
+        <v>0</v>
+      </c>
+      <c r="BA14" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB14">
         <v>2</v>
       </c>
-      <c r="BB14" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC14">
+      <c r="BC14" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD14">
         <v>50</v>
       </c>
-      <c r="BD14">
+      <c r="BE14">
         <v>86</v>
       </c>
-      <c r="BE14" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF14">
+      <c r="BF14" s="2">
         <v>0</v>
       </c>
       <c r="BG14">
@@ -3914,10 +3985,10 @@
       <c r="BJ14">
         <v>0</v>
       </c>
-      <c r="BK14" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL14">
+      <c r="BK14">
+        <v>0</v>
+      </c>
+      <c r="BL14" s="2">
         <v>0</v>
       </c>
       <c r="BM14">
@@ -3942,30 +4013,33 @@
         <v>0</v>
       </c>
       <c r="BT14">
-        <v>1</v>
-      </c>
-      <c r="BU14" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU14">
+        <v>1</v>
       </c>
       <c r="BV14" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW14" s="1">
         <v>40907</v>
       </c>
-      <c r="BW14" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX14" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY14" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -4030,11 +4104,14 @@
       <c r="Z15">
         <v>0</v>
       </c>
+      <c r="AA15" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB15">
         <v>0</v>
       </c>
       <c r="AC15" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -4054,8 +4131,8 @@
       <c r="AI15" s="2">
         <v>0</v>
       </c>
-      <c r="AJ15">
-        <v>0.95</v>
+      <c r="AJ15" s="2">
+        <v>0</v>
       </c>
       <c r="AK15">
         <v>0.95</v>
@@ -4091,7 +4168,7 @@
         <v>0.95</v>
       </c>
       <c r="AV15">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AW15">
         <v>0</v>
@@ -4102,25 +4179,25 @@
       <c r="AY15">
         <v>0</v>
       </c>
-      <c r="AZ15" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA15">
+      <c r="AZ15">
+        <v>0</v>
+      </c>
+      <c r="BA15" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB15">
         <v>3</v>
       </c>
-      <c r="BB15" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC15">
+      <c r="BC15" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD15">
         <v>50</v>
       </c>
-      <c r="BD15">
+      <c r="BE15">
         <v>86</v>
       </c>
-      <c r="BE15" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF15">
+      <c r="BF15" s="2">
         <v>0</v>
       </c>
       <c r="BG15">
@@ -4135,10 +4212,10 @@
       <c r="BJ15">
         <v>0</v>
       </c>
-      <c r="BK15" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL15">
+      <c r="BK15">
+        <v>0</v>
+      </c>
+      <c r="BL15" s="2">
         <v>0</v>
       </c>
       <c r="BM15">
@@ -4163,30 +4240,33 @@
         <v>0</v>
       </c>
       <c r="BT15">
-        <v>1</v>
-      </c>
-      <c r="BU15" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU15">
+        <v>1</v>
       </c>
       <c r="BV15" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW15" s="1">
         <v>40907</v>
       </c>
-      <c r="BW15" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX15" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY15" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -4251,11 +4331,14 @@
       <c r="Z16">
         <v>0</v>
       </c>
+      <c r="AA16" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB16">
         <v>0</v>
       </c>
       <c r="AC16" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -4275,8 +4358,8 @@
       <c r="AI16" s="2">
         <v>0</v>
       </c>
-      <c r="AJ16">
-        <v>1</v>
+      <c r="AJ16" s="2">
+        <v>0</v>
       </c>
       <c r="AK16">
         <v>1</v>
@@ -4312,7 +4395,7 @@
         <v>1</v>
       </c>
       <c r="AV16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW16">
         <v>0</v>
@@ -4323,25 +4406,25 @@
       <c r="AY16">
         <v>0</v>
       </c>
-      <c r="AZ16" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA16">
+      <c r="AZ16">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB16">
         <v>4</v>
       </c>
-      <c r="BB16" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC16">
+      <c r="BC16" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD16">
         <v>50</v>
       </c>
-      <c r="BD16">
+      <c r="BE16">
         <v>86</v>
       </c>
-      <c r="BE16" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF16">
+      <c r="BF16" s="2">
         <v>0</v>
       </c>
       <c r="BG16">
@@ -4356,10 +4439,10 @@
       <c r="BJ16">
         <v>0</v>
       </c>
-      <c r="BK16" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL16">
+      <c r="BK16">
+        <v>0</v>
+      </c>
+      <c r="BL16" s="2">
         <v>0</v>
       </c>
       <c r="BM16">
@@ -4384,30 +4467,33 @@
         <v>0</v>
       </c>
       <c r="BT16">
-        <v>1</v>
-      </c>
-      <c r="BU16" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU16">
+        <v>1</v>
       </c>
       <c r="BV16" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW16" s="1">
         <v>40907</v>
       </c>
-      <c r="BW16" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX16" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY16" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="17" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -4455,7 +4541,7 @@
         <v>2.5</v>
       </c>
       <c r="T17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U17">
         <v>2.5</v>
@@ -4475,11 +4561,14 @@
       <c r="Z17">
         <v>0</v>
       </c>
+      <c r="AA17" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB17">
         <v>0</v>
       </c>
       <c r="AC17" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD17">
         <v>0.05</v>
@@ -4499,8 +4588,8 @@
       <c r="AI17" s="2">
         <v>0</v>
       </c>
-      <c r="AJ17">
-        <v>0.3</v>
+      <c r="AJ17" s="2">
+        <v>0</v>
       </c>
       <c r="AK17">
         <v>0.3</v>
@@ -4536,7 +4625,7 @@
         <v>0.3</v>
       </c>
       <c r="AV17">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AW17">
         <v>0</v>
@@ -4547,25 +4636,25 @@
       <c r="AY17">
         <v>0</v>
       </c>
-      <c r="AZ17" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA17">
+      <c r="AZ17">
+        <v>0</v>
+      </c>
+      <c r="BA17" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB17">
         <v>30</v>
       </c>
-      <c r="BB17" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC17">
+      <c r="BC17" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD17">
         <v>50</v>
       </c>
-      <c r="BD17">
+      <c r="BE17">
         <v>86</v>
       </c>
-      <c r="BE17" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF17">
+      <c r="BF17" s="2">
         <v>0</v>
       </c>
       <c r="BG17">
@@ -4580,10 +4669,10 @@
       <c r="BJ17">
         <v>0</v>
       </c>
-      <c r="BK17" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL17">
+      <c r="BK17">
+        <v>0</v>
+      </c>
+      <c r="BL17" s="2">
         <v>0</v>
       </c>
       <c r="BM17">
@@ -4608,30 +4697,33 @@
         <v>0</v>
       </c>
       <c r="BT17">
-        <v>1</v>
-      </c>
-      <c r="BU17" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU17">
+        <v>1</v>
       </c>
       <c r="BV17" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW17" s="1">
         <v>40907</v>
       </c>
-      <c r="BW17" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX17" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY17" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="18" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -4696,11 +4788,14 @@
       <c r="Z18">
         <v>0</v>
       </c>
+      <c r="AA18" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB18">
         <v>0</v>
       </c>
       <c r="AC18" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD18">
         <v>0.05</v>
@@ -4720,8 +4815,8 @@
       <c r="AI18" s="2">
         <v>0</v>
       </c>
-      <c r="AJ18">
-        <v>0.44</v>
+      <c r="AJ18" s="2">
+        <v>0</v>
       </c>
       <c r="AK18">
         <v>0.44</v>
@@ -4757,7 +4852,7 @@
         <v>0.44</v>
       </c>
       <c r="AV18">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="AW18">
         <v>0</v>
@@ -4768,25 +4863,25 @@
       <c r="AY18">
         <v>0</v>
       </c>
-      <c r="AZ18" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA18">
+      <c r="AZ18">
+        <v>0</v>
+      </c>
+      <c r="BA18" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB18">
         <v>30</v>
       </c>
-      <c r="BB18" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC18">
+      <c r="BC18" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD18">
         <v>50</v>
       </c>
-      <c r="BD18">
+      <c r="BE18">
         <v>86</v>
       </c>
-      <c r="BE18" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF18">
+      <c r="BF18" s="2">
         <v>0</v>
       </c>
       <c r="BG18">
@@ -4801,10 +4896,10 @@
       <c r="BJ18">
         <v>0</v>
       </c>
-      <c r="BK18" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL18">
+      <c r="BK18">
+        <v>0</v>
+      </c>
+      <c r="BL18" s="2">
         <v>0</v>
       </c>
       <c r="BM18">
@@ -4829,30 +4924,33 @@
         <v>0</v>
       </c>
       <c r="BT18">
-        <v>1</v>
-      </c>
-      <c r="BU18" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU18">
+        <v>1</v>
       </c>
       <c r="BV18" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW18" s="1">
         <v>40907</v>
       </c>
-      <c r="BW18" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX18" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY18" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="19" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4917,11 +5015,14 @@
       <c r="Z19">
         <v>0</v>
       </c>
+      <c r="AA19" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB19">
         <v>0</v>
       </c>
       <c r="AC19" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD19">
         <v>0.05</v>
@@ -4941,8 +5042,8 @@
       <c r="AI19" s="2">
         <v>0</v>
       </c>
-      <c r="AJ19">
-        <v>0.44</v>
+      <c r="AJ19" s="2">
+        <v>0</v>
       </c>
       <c r="AK19">
         <v>0.44</v>
@@ -4978,7 +5079,7 @@
         <v>0.44</v>
       </c>
       <c r="AV19">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="AW19">
         <v>0</v>
@@ -4989,25 +5090,25 @@
       <c r="AY19">
         <v>0</v>
       </c>
-      <c r="AZ19" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA19">
+      <c r="AZ19">
+        <v>0</v>
+      </c>
+      <c r="BA19" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB19">
         <v>20</v>
       </c>
-      <c r="BB19" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC19">
+      <c r="BC19" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD19">
         <v>50</v>
       </c>
-      <c r="BD19">
+      <c r="BE19">
         <v>86</v>
       </c>
-      <c r="BE19" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF19">
+      <c r="BF19" s="2">
         <v>0</v>
       </c>
       <c r="BG19">
@@ -5022,10 +5123,10 @@
       <c r="BJ19">
         <v>0</v>
       </c>
-      <c r="BK19" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL19">
+      <c r="BK19">
+        <v>0</v>
+      </c>
+      <c r="BL19" s="2">
         <v>0</v>
       </c>
       <c r="BM19">
@@ -5050,30 +5151,33 @@
         <v>0</v>
       </c>
       <c r="BT19">
-        <v>1</v>
-      </c>
-      <c r="BU19" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU19">
+        <v>1</v>
       </c>
       <c r="BV19" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW19" s="1">
         <v>40907</v>
       </c>
-      <c r="BW19" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX19" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY19" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="20" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -5138,11 +5242,14 @@
       <c r="Z20">
         <v>0</v>
       </c>
+      <c r="AA20" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB20">
         <v>0</v>
       </c>
       <c r="AC20" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD20">
         <v>0</v>
@@ -5162,8 +5269,8 @@
       <c r="AI20" s="2">
         <v>0</v>
       </c>
-      <c r="AJ20">
-        <v>1.05</v>
+      <c r="AJ20" s="2">
+        <v>0</v>
       </c>
       <c r="AK20">
         <v>1.05</v>
@@ -5199,7 +5306,7 @@
         <v>1.05</v>
       </c>
       <c r="AV20">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="AW20">
         <v>0</v>
@@ -5210,25 +5317,25 @@
       <c r="AY20">
         <v>0</v>
       </c>
-      <c r="AZ20" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA20">
-        <v>0</v>
-      </c>
-      <c r="BB20" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC20">
+      <c r="AZ20">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB20">
+        <v>0</v>
+      </c>
+      <c r="BC20" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD20">
         <v>50</v>
       </c>
-      <c r="BD20">
+      <c r="BE20">
         <v>86</v>
       </c>
-      <c r="BE20" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF20">
+      <c r="BF20" s="2">
         <v>0</v>
       </c>
       <c r="BG20">
@@ -5243,10 +5350,10 @@
       <c r="BJ20">
         <v>0</v>
       </c>
-      <c r="BK20" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL20">
+      <c r="BK20">
+        <v>0</v>
+      </c>
+      <c r="BL20" s="2">
         <v>0</v>
       </c>
       <c r="BM20">
@@ -5271,30 +5378,33 @@
         <v>0</v>
       </c>
       <c r="BT20">
-        <v>1</v>
-      </c>
-      <c r="BU20" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU20">
+        <v>1</v>
       </c>
       <c r="BV20" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW20" s="1">
         <v>40907</v>
       </c>
-      <c r="BW20" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX20" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY20" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="21" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -5359,11 +5469,14 @@
       <c r="Z21">
         <v>0</v>
       </c>
+      <c r="AA21" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB21">
         <v>0</v>
       </c>
       <c r="AC21" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD21">
         <v>0</v>
@@ -5383,45 +5496,45 @@
       <c r="AI21" s="2">
         <v>0</v>
       </c>
-      <c r="AJ21">
+      <c r="AJ21" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK21">
         <v>0.85</v>
       </c>
-      <c r="AK21">
+      <c r="AL21">
         <v>0.5</v>
       </c>
-      <c r="AL21">
+      <c r="AM21">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AM21">
+      <c r="AN21">
         <v>0.4</v>
       </c>
-      <c r="AN21">
+      <c r="AO21">
         <v>0.8</v>
       </c>
-      <c r="AO21">
+      <c r="AP21">
         <v>1.2</v>
       </c>
-      <c r="AP21">
+      <c r="AQ21">
         <v>0.85</v>
       </c>
-      <c r="AQ21">
+      <c r="AR21">
         <v>0.5</v>
       </c>
-      <c r="AR21">
+      <c r="AS21">
         <v>0.28999999999999998</v>
       </c>
-      <c r="AS21">
+      <c r="AT21">
         <v>0.4</v>
       </c>
-      <c r="AT21">
+      <c r="AU21">
         <v>0.8</v>
       </c>
-      <c r="AU21">
+      <c r="AV21">
         <v>1.2</v>
       </c>
-      <c r="AV21">
-        <v>0</v>
-      </c>
       <c r="AW21">
         <v>0</v>
       </c>
@@ -5431,25 +5544,25 @@
       <c r="AY21">
         <v>0</v>
       </c>
-      <c r="AZ21" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA21">
-        <v>0</v>
-      </c>
-      <c r="BB21" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC21">
+      <c r="AZ21">
+        <v>0</v>
+      </c>
+      <c r="BA21" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB21">
+        <v>0</v>
+      </c>
+      <c r="BC21" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD21">
         <v>50</v>
       </c>
-      <c r="BD21">
+      <c r="BE21">
         <v>86</v>
       </c>
-      <c r="BE21" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF21">
+      <c r="BF21" s="2">
         <v>0</v>
       </c>
       <c r="BG21">
@@ -5464,10 +5577,10 @@
       <c r="BJ21">
         <v>0</v>
       </c>
-      <c r="BK21" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL21">
+      <c r="BK21">
+        <v>0</v>
+      </c>
+      <c r="BL21" s="2">
         <v>0</v>
       </c>
       <c r="BM21">
@@ -5492,30 +5605,33 @@
         <v>0</v>
       </c>
       <c r="BT21">
-        <v>1</v>
-      </c>
-      <c r="BU21" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU21">
+        <v>1</v>
       </c>
       <c r="BV21" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW21" s="1">
         <v>40907</v>
       </c>
-      <c r="BW21" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX21" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY21" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="22" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -5580,11 +5696,14 @@
       <c r="Z22">
         <v>0</v>
       </c>
+      <c r="AA22" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB22">
         <v>0</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD22">
         <v>0.05</v>
@@ -5604,8 +5723,8 @@
       <c r="AI22" s="2">
         <v>0</v>
       </c>
-      <c r="AJ22">
-        <v>0.3</v>
+      <c r="AJ22" s="2">
+        <v>0</v>
       </c>
       <c r="AK22">
         <v>0.3</v>
@@ -5641,7 +5760,7 @@
         <v>0.3</v>
       </c>
       <c r="AV22">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AW22">
         <v>0</v>
@@ -5652,25 +5771,25 @@
       <c r="AY22">
         <v>0</v>
       </c>
-      <c r="AZ22" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA22">
+      <c r="AZ22">
+        <v>0</v>
+      </c>
+      <c r="BA22" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB22">
         <v>30</v>
       </c>
-      <c r="BB22" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC22">
+      <c r="BC22" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD22">
         <v>50</v>
       </c>
-      <c r="BD22">
+      <c r="BE22">
         <v>86</v>
       </c>
-      <c r="BE22" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF22">
+      <c r="BF22" s="2">
         <v>0</v>
       </c>
       <c r="BG22">
@@ -5685,10 +5804,10 @@
       <c r="BJ22">
         <v>0</v>
       </c>
-      <c r="BK22" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL22">
+      <c r="BK22">
+        <v>0</v>
+      </c>
+      <c r="BL22" s="2">
         <v>0</v>
       </c>
       <c r="BM22">
@@ -5713,30 +5832,33 @@
         <v>0</v>
       </c>
       <c r="BT22">
-        <v>1</v>
-      </c>
-      <c r="BU22" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU22">
+        <v>1</v>
       </c>
       <c r="BV22" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW22" s="1">
         <v>40907</v>
       </c>
-      <c r="BW22" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX22" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY22" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="23" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -5801,11 +5923,14 @@
       <c r="Z23">
         <v>0</v>
       </c>
+      <c r="AA23" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB23">
         <v>0</v>
       </c>
       <c r="AC23" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD23">
         <v>0.05</v>
@@ -5825,8 +5950,8 @@
       <c r="AI23" s="2">
         <v>0</v>
       </c>
-      <c r="AJ23">
-        <v>0.33</v>
+      <c r="AJ23" s="2">
+        <v>0</v>
       </c>
       <c r="AK23">
         <v>0.33</v>
@@ -5862,7 +5987,7 @@
         <v>0.33</v>
       </c>
       <c r="AV23">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AW23">
         <v>0</v>
@@ -5873,25 +5998,25 @@
       <c r="AY23">
         <v>0</v>
       </c>
-      <c r="AZ23" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA23">
+      <c r="AZ23">
+        <v>0</v>
+      </c>
+      <c r="BA23" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB23">
         <v>30</v>
       </c>
-      <c r="BB23" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC23">
+      <c r="BC23" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD23">
         <v>50</v>
       </c>
-      <c r="BD23">
+      <c r="BE23">
         <v>86</v>
       </c>
-      <c r="BE23" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF23">
+      <c r="BF23" s="2">
         <v>0</v>
       </c>
       <c r="BG23">
@@ -5906,10 +6031,10 @@
       <c r="BJ23">
         <v>0</v>
       </c>
-      <c r="BK23" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL23">
+      <c r="BK23">
+        <v>0</v>
+      </c>
+      <c r="BL23" s="2">
         <v>0</v>
       </c>
       <c r="BM23">
@@ -5934,30 +6059,33 @@
         <v>0</v>
       </c>
       <c r="BT23">
-        <v>1</v>
-      </c>
-      <c r="BU23" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU23">
+        <v>1</v>
       </c>
       <c r="BV23" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW23" s="1">
         <v>40907</v>
       </c>
-      <c r="BW23" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX23" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY23" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="24" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -6022,11 +6150,14 @@
       <c r="Z24">
         <v>0</v>
       </c>
+      <c r="AA24" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB24">
         <v>0</v>
       </c>
       <c r="AC24" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD24">
         <v>0.05</v>
@@ -6046,8 +6177,8 @@
       <c r="AI24" s="2">
         <v>0</v>
       </c>
-      <c r="AJ24">
-        <v>0.33</v>
+      <c r="AJ24" s="2">
+        <v>0</v>
       </c>
       <c r="AK24">
         <v>0.33</v>
@@ -6083,7 +6214,7 @@
         <v>0.33</v>
       </c>
       <c r="AV24">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="AW24">
         <v>0</v>
@@ -6094,25 +6225,25 @@
       <c r="AY24">
         <v>0</v>
       </c>
-      <c r="AZ24" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA24">
+      <c r="AZ24">
+        <v>0</v>
+      </c>
+      <c r="BA24" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB24">
         <v>30</v>
       </c>
-      <c r="BB24" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC24">
+      <c r="BC24" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD24">
         <v>50</v>
       </c>
-      <c r="BD24">
+      <c r="BE24">
         <v>86</v>
       </c>
-      <c r="BE24" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF24">
+      <c r="BF24" s="2">
         <v>0</v>
       </c>
       <c r="BG24">
@@ -6127,10 +6258,10 @@
       <c r="BJ24">
         <v>0</v>
       </c>
-      <c r="BK24" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL24">
+      <c r="BK24">
+        <v>0</v>
+      </c>
+      <c r="BL24" s="2">
         <v>0</v>
       </c>
       <c r="BM24">
@@ -6155,30 +6286,33 @@
         <v>0</v>
       </c>
       <c r="BT24">
-        <v>1</v>
-      </c>
-      <c r="BU24" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU24">
+        <v>1</v>
       </c>
       <c r="BV24" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW24" s="1">
         <v>40907</v>
       </c>
-      <c r="BW24" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX24" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY24" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="25" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -6244,13 +6378,13 @@
         <v>2</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB25" s="2">
         <v>0</v>
       </c>
       <c r="AC25" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD25" s="2">
         <v>0</v>
@@ -6271,7 +6405,7 @@
         <v>0</v>
       </c>
       <c r="AJ25" s="2">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="AK25" s="2">
         <v>0.85</v>
@@ -6307,7 +6441,7 @@
         <v>0.85</v>
       </c>
       <c r="AV25" s="2">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="AW25" s="2">
         <v>0</v>
@@ -6318,24 +6452,24 @@
       <c r="AY25" s="2">
         <v>0</v>
       </c>
-      <c r="AZ25" s="3">
-        <v>40543</v>
-      </c>
-      <c r="BA25" s="2">
-        <v>1</v>
-      </c>
-      <c r="BB25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC25" s="2">
+      <c r="AZ25" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA25" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BB25" s="2">
+        <v>1</v>
+      </c>
+      <c r="BC25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD25" s="2">
         <v>50</v>
       </c>
-      <c r="BD25" s="2">
+      <c r="BE25" s="2">
         <v>86</v>
       </c>
-      <c r="BE25" s="2">
-        <v>0</v>
-      </c>
       <c r="BF25" s="2">
         <v>0</v>
       </c>
@@ -6379,30 +6513,33 @@
         <v>0</v>
       </c>
       <c r="BT25" s="2">
-        <v>1</v>
-      </c>
-      <c r="BU25" s="3">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU25" s="2">
+        <v>1</v>
       </c>
       <c r="BV25" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BW25" s="3">
         <v>40907</v>
       </c>
-      <c r="BW25" s="3">
-        <v>40543</v>
-      </c>
       <c r="BX25" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BY25" s="3">
         <v>40907</v>
       </c>
     </row>
-    <row r="26" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="2">
         <v>0</v>
@@ -6468,13 +6605,13 @@
         <v>0</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AB26" s="2">
         <v>1.2465753420000001</v>
       </c>
       <c r="AC26" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD26" s="2">
         <v>0</v>
@@ -6495,7 +6632,7 @@
         <v>0</v>
       </c>
       <c r="AJ26" s="2">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="AK26" s="2">
         <v>0.95</v>
@@ -6531,7 +6668,7 @@
         <v>0.95</v>
       </c>
       <c r="AV26" s="2">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="AW26" s="2">
         <v>0</v>
@@ -6542,24 +6679,24 @@
       <c r="AY26" s="2">
         <v>0</v>
       </c>
-      <c r="AZ26" s="3">
-        <v>40543</v>
-      </c>
-      <c r="BA26" s="2">
+      <c r="AZ26" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA26" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BB26" s="2">
         <v>10</v>
       </c>
-      <c r="BB26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC26" s="2">
+      <c r="BC26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD26" s="2">
         <v>50</v>
       </c>
-      <c r="BD26" s="2">
+      <c r="BE26" s="2">
         <v>86</v>
       </c>
-      <c r="BE26" s="2">
-        <v>0</v>
-      </c>
       <c r="BF26" s="2">
         <v>0</v>
       </c>
@@ -6603,30 +6740,33 @@
         <v>0</v>
       </c>
       <c r="BT26" s="2">
-        <v>1</v>
-      </c>
-      <c r="BU26" s="3">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU26" s="2">
+        <v>1</v>
       </c>
       <c r="BV26" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BW26" s="3">
         <v>40907</v>
       </c>
-      <c r="BW26" s="3">
-        <v>40543</v>
-      </c>
       <c r="BX26" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BY26" s="3">
         <v>40907</v>
       </c>
     </row>
-    <row r="27" spans="1:76" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -6674,7 +6814,7 @@
         <v>2</v>
       </c>
       <c r="S27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U27">
         <v>2</v>
@@ -6694,11 +6834,14 @@
       <c r="Z27">
         <v>5</v>
       </c>
+      <c r="AA27" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB27">
         <v>0</v>
       </c>
       <c r="AC27" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD27">
         <v>0</v>
@@ -6718,7 +6861,7 @@
       <c r="AI27" s="2">
         <v>0</v>
       </c>
-      <c r="AJ27">
+      <c r="AJ27" s="2">
         <v>0</v>
       </c>
       <c r="AK27">
@@ -6755,56 +6898,56 @@
         <v>0</v>
       </c>
       <c r="AV27">
+        <v>0</v>
+      </c>
+      <c r="AW27">
         <v>0.5</v>
       </c>
-      <c r="AW27">
+      <c r="AX27">
         <v>1.25</v>
       </c>
-      <c r="AX27">
+      <c r="AY27">
         <v>0.88</v>
       </c>
-      <c r="AY27">
+      <c r="AZ27">
         <v>0.31</v>
       </c>
-      <c r="AZ27" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA27">
+      <c r="BA27" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB27">
         <v>6</v>
       </c>
-      <c r="BB27" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC27">
+      <c r="BC27" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD27">
         <v>50</v>
       </c>
-      <c r="BD27">
+      <c r="BE27">
         <v>86</v>
       </c>
-      <c r="BE27" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF27">
+      <c r="BF27" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG27">
         <v>76</v>
       </c>
-      <c r="BG27">
+      <c r="BH27">
         <v>107</v>
       </c>
-      <c r="BH27">
+      <c r="BI27">
         <v>334</v>
       </c>
-      <c r="BI27">
+      <c r="BJ27">
         <v>152</v>
       </c>
-      <c r="BJ27">
+      <c r="BK27">
         <v>61</v>
       </c>
-      <c r="BK27" s="2">
+      <c r="BL27" s="2">
         <v>608</v>
       </c>
-      <c r="BL27">
-        <v>0</v>
-      </c>
       <c r="BM27">
         <v>0</v>
       </c>
@@ -6827,30 +6970,33 @@
         <v>0</v>
       </c>
       <c r="BT27">
-        <v>1</v>
-      </c>
-      <c r="BU27" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU27">
+        <v>1</v>
       </c>
       <c r="BV27" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW27" s="1">
         <v>40907</v>
       </c>
-      <c r="BW27" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX27" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY27" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="28" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -6915,11 +7061,14 @@
       <c r="Z28">
         <v>0</v>
       </c>
+      <c r="AA28" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB28">
         <v>0</v>
       </c>
       <c r="AC28" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD28">
         <v>0</v>
@@ -6939,8 +7088,8 @@
       <c r="AI28" s="2">
         <v>0</v>
       </c>
-      <c r="AJ28">
-        <v>0.98</v>
+      <c r="AJ28" s="2">
+        <v>0</v>
       </c>
       <c r="AK28">
         <v>0.98</v>
@@ -6976,7 +7125,7 @@
         <v>0.98</v>
       </c>
       <c r="AV28">
-        <v>0</v>
+        <v>0.98</v>
       </c>
       <c r="AW28">
         <v>0</v>
@@ -6987,25 +7136,25 @@
       <c r="AY28">
         <v>0</v>
       </c>
-      <c r="AZ28" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA28">
+      <c r="AZ28">
+        <v>0</v>
+      </c>
+      <c r="BA28" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB28">
         <v>4</v>
       </c>
-      <c r="BB28" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC28">
+      <c r="BC28" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD28">
         <v>50</v>
       </c>
-      <c r="BD28">
+      <c r="BE28">
         <v>86</v>
       </c>
-      <c r="BE28" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF28">
+      <c r="BF28" s="2">
         <v>0</v>
       </c>
       <c r="BG28">
@@ -7020,10 +7169,10 @@
       <c r="BJ28">
         <v>0</v>
       </c>
-      <c r="BK28" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL28">
+      <c r="BK28">
+        <v>0</v>
+      </c>
+      <c r="BL28" s="2">
         <v>0</v>
       </c>
       <c r="BM28">
@@ -7048,30 +7197,33 @@
         <v>0</v>
       </c>
       <c r="BT28">
-        <v>1</v>
-      </c>
-      <c r="BU28" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU28">
+        <v>1</v>
       </c>
       <c r="BV28" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW28" s="1">
         <v>40907</v>
       </c>
-      <c r="BW28" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX28" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY28" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="29" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -7136,11 +7288,14 @@
       <c r="Z29">
         <v>0</v>
       </c>
+      <c r="AA29" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB29">
         <v>0</v>
       </c>
       <c r="AC29" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD29">
         <v>0.05</v>
@@ -7160,8 +7315,8 @@
       <c r="AI29" s="2">
         <v>0</v>
       </c>
-      <c r="AJ29">
-        <v>0.69</v>
+      <c r="AJ29" s="2">
+        <v>0</v>
       </c>
       <c r="AK29">
         <v>0.69</v>
@@ -7197,7 +7352,7 @@
         <v>0.69</v>
       </c>
       <c r="AV29">
-        <v>0</v>
+        <v>0.69</v>
       </c>
       <c r="AW29">
         <v>0</v>
@@ -7208,25 +7363,25 @@
       <c r="AY29">
         <v>0</v>
       </c>
-      <c r="AZ29" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA29">
+      <c r="AZ29">
+        <v>0</v>
+      </c>
+      <c r="BA29" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB29">
         <v>4</v>
       </c>
-      <c r="BB29" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC29">
+      <c r="BC29" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD29">
         <v>50</v>
       </c>
-      <c r="BD29">
+      <c r="BE29">
         <v>86</v>
       </c>
-      <c r="BE29" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF29">
+      <c r="BF29" s="2">
         <v>0</v>
       </c>
       <c r="BG29">
@@ -7241,10 +7396,10 @@
       <c r="BJ29">
         <v>0</v>
       </c>
-      <c r="BK29" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL29">
+      <c r="BK29">
+        <v>0</v>
+      </c>
+      <c r="BL29" s="2">
         <v>0</v>
       </c>
       <c r="BM29">
@@ -7269,30 +7424,33 @@
         <v>0</v>
       </c>
       <c r="BT29">
-        <v>1</v>
-      </c>
-      <c r="BU29" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU29">
+        <v>1</v>
       </c>
       <c r="BV29" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW29" s="1">
         <v>40907</v>
       </c>
-      <c r="BW29" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX29" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY29" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="30" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -7357,11 +7515,14 @@
       <c r="Z30">
         <v>0</v>
       </c>
+      <c r="AA30" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB30">
         <v>0</v>
       </c>
       <c r="AC30" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD30">
         <v>0</v>
@@ -7381,8 +7542,8 @@
       <c r="AI30" s="2">
         <v>0</v>
       </c>
-      <c r="AJ30">
-        <v>1.07</v>
+      <c r="AJ30" s="2">
+        <v>0</v>
       </c>
       <c r="AK30">
         <v>1.07</v>
@@ -7418,7 +7579,7 @@
         <v>1.07</v>
       </c>
       <c r="AV30">
-        <v>0</v>
+        <v>1.07</v>
       </c>
       <c r="AW30">
         <v>0</v>
@@ -7429,25 +7590,25 @@
       <c r="AY30">
         <v>0</v>
       </c>
-      <c r="AZ30" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA30">
+      <c r="AZ30">
+        <v>0</v>
+      </c>
+      <c r="BA30" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB30">
         <v>4</v>
       </c>
-      <c r="BB30" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC30">
+      <c r="BC30" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD30">
         <v>50</v>
       </c>
-      <c r="BD30">
+      <c r="BE30">
         <v>86</v>
       </c>
-      <c r="BE30" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF30">
+      <c r="BF30" s="2">
         <v>0</v>
       </c>
       <c r="BG30">
@@ -7462,10 +7623,10 @@
       <c r="BJ30">
         <v>0</v>
       </c>
-      <c r="BK30" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL30">
+      <c r="BK30">
+        <v>0</v>
+      </c>
+      <c r="BL30" s="2">
         <v>0</v>
       </c>
       <c r="BM30">
@@ -7490,30 +7651,33 @@
         <v>0</v>
       </c>
       <c r="BT30">
-        <v>1</v>
-      </c>
-      <c r="BU30" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU30">
+        <v>1</v>
       </c>
       <c r="BV30" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW30" s="1">
         <v>40907</v>
       </c>
-      <c r="BW30" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX30" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY30" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="31" spans="1:76" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -7578,11 +7742,14 @@
       <c r="Z31">
         <v>0</v>
       </c>
+      <c r="AA31" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="AB31">
         <v>0</v>
       </c>
       <c r="AC31" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -7602,8 +7769,8 @@
       <c r="AI31" s="2">
         <v>0</v>
       </c>
-      <c r="AJ31">
-        <v>1.05</v>
+      <c r="AJ31" s="2">
+        <v>0</v>
       </c>
       <c r="AK31">
         <v>1.05</v>
@@ -7639,7 +7806,7 @@
         <v>1.05</v>
       </c>
       <c r="AV31">
-        <v>0</v>
+        <v>1.05</v>
       </c>
       <c r="AW31">
         <v>0</v>
@@ -7650,25 +7817,25 @@
       <c r="AY31">
         <v>0</v>
       </c>
-      <c r="AZ31" s="1">
-        <v>40543</v>
-      </c>
-      <c r="BA31">
-        <v>0</v>
-      </c>
-      <c r="BB31" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC31">
+      <c r="AZ31">
+        <v>0</v>
+      </c>
+      <c r="BA31" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BB31">
+        <v>0</v>
+      </c>
+      <c r="BC31" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD31">
         <v>50</v>
       </c>
-      <c r="BD31">
+      <c r="BE31">
         <v>86</v>
       </c>
-      <c r="BE31" s="2">
-        <v>0</v>
-      </c>
-      <c r="BF31">
+      <c r="BF31" s="2">
         <v>0</v>
       </c>
       <c r="BG31">
@@ -7683,10 +7850,10 @@
       <c r="BJ31">
         <v>0</v>
       </c>
-      <c r="BK31" s="2">
-        <v>0</v>
-      </c>
-      <c r="BL31">
+      <c r="BK31">
+        <v>0</v>
+      </c>
+      <c r="BL31" s="2">
         <v>0</v>
       </c>
       <c r="BM31">
@@ -7711,30 +7878,33 @@
         <v>0</v>
       </c>
       <c r="BT31">
-        <v>1</v>
-      </c>
-      <c r="BU31" s="1">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU31">
+        <v>1</v>
       </c>
       <c r="BV31" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BW31" s="1">
         <v>40907</v>
       </c>
-      <c r="BW31" s="1">
-        <v>40543</v>
-      </c>
       <c r="BX31" s="1">
+        <v>40543</v>
+      </c>
+      <c r="BY31" s="1">
         <v>40907</v>
       </c>
     </row>
-    <row r="32" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D32" s="2">
         <v>0</v>
@@ -7782,7 +7952,7 @@
         <v>2</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U32" s="2">
         <v>2</v>
@@ -7803,13 +7973,13 @@
         <v>4</v>
       </c>
       <c r="AA32" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB32" s="2">
         <v>0</v>
       </c>
       <c r="AC32" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD32" s="2">
         <v>0</v>
@@ -7866,57 +8036,57 @@
         <v>0</v>
       </c>
       <c r="AV32" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW32" s="2">
         <v>0.5</v>
       </c>
-      <c r="AW32" s="2">
+      <c r="AX32" s="2">
         <v>1.25</v>
       </c>
-      <c r="AX32" s="2">
+      <c r="AY32" s="2">
         <v>0.88</v>
       </c>
-      <c r="AY32" s="2">
+      <c r="AZ32" s="2">
         <v>0.31</v>
       </c>
-      <c r="AZ32" s="3">
-        <v>40543</v>
-      </c>
-      <c r="BA32" s="2">
+      <c r="BA32" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BB32" s="2">
         <v>5</v>
       </c>
-      <c r="BB32" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC32" s="2">
+      <c r="BC32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD32" s="2">
         <v>50</v>
       </c>
-      <c r="BD32" s="2">
+      <c r="BE32" s="2">
         <v>86</v>
       </c>
-      <c r="BE32" s="2">
+      <c r="BF32" s="2">
         <v>-365</v>
       </c>
-      <c r="BF32" s="2">
+      <c r="BG32" s="2">
         <v>76</v>
       </c>
-      <c r="BG32" s="2">
+      <c r="BH32" s="2">
         <v>107</v>
       </c>
-      <c r="BH32" s="2">
+      <c r="BI32" s="2">
         <v>334</v>
       </c>
-      <c r="BI32" s="2">
+      <c r="BJ32" s="2">
         <v>152</v>
       </c>
-      <c r="BJ32" s="2">
+      <c r="BK32" s="2">
         <v>61</v>
       </c>
-      <c r="BK32" s="2">
-        <f>SUM(BF32:BJ32)-122</f>
+      <c r="BL32" s="2">
+        <f>SUM(BG32:BK32)-122</f>
         <v>608</v>
       </c>
-      <c r="BL32" s="2">
-        <v>0</v>
-      </c>
       <c r="BM32" s="2">
         <v>0</v>
       </c>
@@ -7939,30 +8109,33 @@
         <v>0</v>
       </c>
       <c r="BT32" s="2">
-        <v>1</v>
-      </c>
-      <c r="BU32" s="3">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU32" s="2">
+        <v>1</v>
       </c>
       <c r="BV32" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BW32" s="3">
         <v>40907</v>
       </c>
-      <c r="BW32" s="3">
-        <v>40543</v>
-      </c>
       <c r="BX32" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BY32" s="3">
         <v>40907</v>
       </c>
     </row>
-    <row r="33" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>42</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D33" s="2">
         <v>0</v>
@@ -8010,7 +8183,7 @@
         <v>2</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="U33" s="2">
         <v>2</v>
@@ -8031,13 +8204,13 @@
         <v>4</v>
       </c>
       <c r="AA33" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB33" s="2">
         <v>0</v>
       </c>
       <c r="AC33" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AD33" s="2">
         <v>0</v>
@@ -8094,56 +8267,56 @@
         <v>0</v>
       </c>
       <c r="AV33" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW33" s="2">
         <v>0.5</v>
       </c>
-      <c r="AW33" s="2">
+      <c r="AX33" s="2">
         <v>1.25</v>
       </c>
-      <c r="AX33" s="2">
+      <c r="AY33" s="2">
         <v>0.88</v>
       </c>
-      <c r="AY33" s="2">
+      <c r="AZ33" s="2">
         <v>0.31</v>
       </c>
-      <c r="AZ33" s="3">
-        <v>40543</v>
-      </c>
-      <c r="BA33" s="2">
+      <c r="BA33" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BB33" s="2">
         <v>5</v>
       </c>
-      <c r="BB33" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="BC33" s="2">
+      <c r="BC33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="BD33" s="2">
         <v>50</v>
       </c>
-      <c r="BD33" s="2">
+      <c r="BE33" s="2">
         <v>86</v>
       </c>
-      <c r="BE33" s="2">
-        <v>0</v>
-      </c>
       <c r="BF33" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG33" s="2">
         <v>76</v>
       </c>
-      <c r="BG33" s="2">
+      <c r="BH33" s="2">
         <v>107</v>
       </c>
-      <c r="BH33" s="2">
+      <c r="BI33" s="2">
         <v>334</v>
       </c>
-      <c r="BI33" s="2">
+      <c r="BJ33" s="2">
         <v>152</v>
       </c>
-      <c r="BJ33" s="2">
+      <c r="BK33" s="2">
         <v>61</v>
       </c>
-      <c r="BK33" s="2">
+      <c r="BL33" s="2">
         <v>608</v>
       </c>
-      <c r="BL33" s="2">
-        <v>0</v>
-      </c>
       <c r="BM33" s="2">
         <v>0</v>
       </c>
@@ -8166,18 +8339,21 @@
         <v>0</v>
       </c>
       <c r="BT33" s="2">
-        <v>1</v>
-      </c>
-      <c r="BU33" s="3">
-        <v>40543</v>
+        <v>0</v>
+      </c>
+      <c r="BU33" s="2">
+        <v>1</v>
       </c>
       <c r="BV33" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BW33" s="3">
         <v>40907</v>
       </c>
-      <c r="BW33" s="3">
-        <v>40543</v>
-      </c>
       <c r="BX33" s="3">
+        <v>40543</v>
+      </c>
+      <c r="BY33" s="3">
         <v>40907</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update executable; add toy example to Maui showing direct soil moisture (septic) additions via table entry.
</commit_message>
<xml_diff>
--- a/maui/std_input/Landuse_lookup_maui.xlsx
+++ b/maui/std_input/Landuse_lookup_maui.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smwesten/SMWData/Static/Source_Code/swb2_examples/maui/std_input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SMWData\Git_repos\swb2_examples\maui\std_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LU_lookup_Engott_v3_6.txt" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -230,9 +230,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Cooley, Keith R., and Leonard J. Lane. ÒModified Runoff Curve Numbers for Sugarcane and Pineapple Fields in Hawaii.Ó Journal of Soil and Water Conservation 37, no. 5 (1982): 295Ð98.</t>
-  </si>
-  <si>
     <t>PE - P demand</t>
   </si>
   <si>
@@ -383,7 +380,10 @@
     <t>Annual_direct_net_infiltration</t>
   </si>
   <si>
-    <t>Annual_esptic_discharge</t>
+    <t>Annual_septic_discharge</t>
+  </si>
+  <si>
+    <t>Cooley, Keith R., and Leonard J. Lane. Modified Runoff Curve Numbers for Sugarcane and Pineapple Fields in Hawaii. Journal of Soil and Water Conservation 37, no. 5 (1982): 295-98.</t>
   </si>
 </sst>
 </file>
@@ -826,20 +826,21 @@
   <dimension ref="A1:BY33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AJ12" sqref="AJ12"/>
+      <selection pane="bottomRight" activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.125" customWidth="1"/>
+    <col min="19" max="19" width="155.125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.5" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="32.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.6640625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="32.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.625" style="1" customWidth="1"/>
     <col min="54" max="54" width="17.5" bestFit="1" customWidth="1"/>
     <col min="74" max="77" width="11" style="1"/>
   </cols>
@@ -870,16 +871,16 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
         <v>112</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>113</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>114</v>
-      </c>
-      <c r="L1" t="s">
-        <v>115</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -930,7 +931,7 @@
         <v>23</v>
       </c>
       <c r="AC1" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AD1" t="s">
         <v>24</v>
@@ -945,13 +946,13 @@
         <v>27</v>
       </c>
       <c r="AH1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>117</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>118</v>
       </c>
       <c r="AK1" t="s">
         <v>28</v>
@@ -1002,7 +1003,7 @@
         <v>43</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="BB1" t="s">
         <v>44</v>
@@ -1017,7 +1018,7 @@
         <v>47</v>
       </c>
       <c r="BF1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="BG1" t="s">
         <v>48</v>
@@ -1035,7 +1036,7 @@
         <v>52</v>
       </c>
       <c r="BL1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="BM1" t="s">
         <v>53</v>
@@ -1071,10 +1072,10 @@
         <v>63</v>
       </c>
       <c r="BX1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="BY1" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="BY1" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:77" x14ac:dyDescent="0.25">
@@ -1151,13 +1152,13 @@
         <v>0</v>
       </c>
       <c r="AA2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AB2">
         <v>0</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD2">
         <v>0</v>
@@ -1304,12 +1305,12 @@
         <v>40907</v>
       </c>
     </row>
-    <row r="3" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>65</v>
@@ -1360,7 +1361,7 @@
         <v>1.5</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="U3" s="2">
         <v>1.5</v>
@@ -1381,13 +1382,13 @@
         <v>6</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB3" s="2">
         <v>0</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AD3" s="2">
         <v>0</v>
@@ -1539,7 +1540,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>65</v>
@@ -1608,13 +1609,13 @@
         <v>8</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB4" s="2">
         <v>0</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AD4" s="2">
         <v>0</v>
@@ -1766,7 +1767,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>65</v>
@@ -1835,13 +1836,13 @@
         <v>10</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB5" s="2">
         <v>0</v>
       </c>
       <c r="AC5" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AD5" s="2">
         <v>0</v>
@@ -1993,7 +1994,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
         <v>65</v>
@@ -2062,13 +2063,13 @@
         <v>0</v>
       </c>
       <c r="AA6" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB6">
         <v>0</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -2220,7 +2221,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
         <v>65</v>
@@ -2289,13 +2290,13 @@
         <v>0</v>
       </c>
       <c r="AA7" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB7">
         <v>0</v>
       </c>
       <c r="AC7" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD7">
         <v>0</v>
@@ -2447,7 +2448,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
         <v>65</v>
@@ -2516,13 +2517,13 @@
         <v>0</v>
       </c>
       <c r="AA8" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB8">
         <v>0</v>
       </c>
       <c r="AC8" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD8">
         <v>0</v>
@@ -2674,7 +2675,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9">
         <v>18</v>
@@ -2743,13 +2744,13 @@
         <v>0</v>
       </c>
       <c r="AA9" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB9">
         <v>0</v>
       </c>
       <c r="AC9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD9">
         <v>0</v>
@@ -2901,7 +2902,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="2">
         <v>58</v>
@@ -2970,13 +2971,13 @@
         <v>1</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB10" s="2">
         <v>0</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AD10" s="2">
         <v>0</v>
@@ -3128,7 +3129,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="2">
         <v>84</v>
@@ -3197,13 +3198,13 @@
         <v>1</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB11" s="2">
         <v>0</v>
       </c>
       <c r="AC11" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AD11" s="2">
         <v>0</v>
@@ -3355,7 +3356,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
@@ -3424,13 +3425,13 @@
         <v>0</v>
       </c>
       <c r="AA12" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB12">
         <v>0</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD12">
         <v>0</v>
@@ -3582,7 +3583,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C13" t="s">
         <v>65</v>
@@ -3651,13 +3652,13 @@
         <v>0</v>
       </c>
       <c r="AA13" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB13">
         <v>0</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD13">
         <v>0</v>
@@ -3809,7 +3810,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
         <v>65</v>
@@ -3878,13 +3879,13 @@
         <v>0</v>
       </c>
       <c r="AA14" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB14">
         <v>0</v>
       </c>
       <c r="AC14" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD14">
         <v>0</v>
@@ -4036,7 +4037,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
         <v>65</v>
@@ -4105,13 +4106,13 @@
         <v>0</v>
       </c>
       <c r="AA15" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB15">
         <v>0</v>
       </c>
       <c r="AC15" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD15">
         <v>0</v>
@@ -4263,7 +4264,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" t="s">
         <v>65</v>
@@ -4332,13 +4333,13 @@
         <v>0</v>
       </c>
       <c r="AA16" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB16">
         <v>0</v>
       </c>
       <c r="AC16" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -4490,7 +4491,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17" t="s">
         <v>65</v>
@@ -4541,7 +4542,7 @@
         <v>2.5</v>
       </c>
       <c r="T17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U17">
         <v>2.5</v>
@@ -4562,13 +4563,13 @@
         <v>0</v>
       </c>
       <c r="AA17" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB17">
         <v>0</v>
       </c>
       <c r="AC17" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD17">
         <v>0.05</v>
@@ -4720,7 +4721,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" t="s">
         <v>65</v>
@@ -4789,13 +4790,13 @@
         <v>0</v>
       </c>
       <c r="AA18" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB18">
         <v>0</v>
       </c>
       <c r="AC18" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD18">
         <v>0.05</v>
@@ -4947,7 +4948,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
         <v>65</v>
@@ -5016,13 +5017,13 @@
         <v>0</v>
       </c>
       <c r="AA19" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB19">
         <v>0</v>
       </c>
       <c r="AC19" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD19">
         <v>0.05</v>
@@ -5174,7 +5175,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C20" t="s">
         <v>65</v>
@@ -5243,13 +5244,13 @@
         <v>0</v>
       </c>
       <c r="AA20" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB20">
         <v>0</v>
       </c>
       <c r="AC20" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD20">
         <v>0</v>
@@ -5401,7 +5402,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
         <v>65</v>
@@ -5470,13 +5471,13 @@
         <v>0</v>
       </c>
       <c r="AA21" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB21">
         <v>0</v>
       </c>
       <c r="AC21" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD21">
         <v>0</v>
@@ -5628,7 +5629,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C22" t="s">
         <v>65</v>
@@ -5697,13 +5698,13 @@
         <v>0</v>
       </c>
       <c r="AA22" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB22">
         <v>0</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD22">
         <v>0.05</v>
@@ -5855,7 +5856,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
         <v>65</v>
@@ -5924,13 +5925,13 @@
         <v>0</v>
       </c>
       <c r="AA23" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB23">
         <v>0</v>
       </c>
       <c r="AC23" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD23">
         <v>0.05</v>
@@ -6082,7 +6083,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" t="s">
         <v>65</v>
@@ -6151,13 +6152,13 @@
         <v>0</v>
       </c>
       <c r="AA24" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB24">
         <v>0</v>
       </c>
       <c r="AC24" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD24">
         <v>0.05</v>
@@ -6309,7 +6310,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>65</v>
@@ -6378,13 +6379,13 @@
         <v>2</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB25" s="2">
         <v>0</v>
       </c>
       <c r="AC25" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AD25" s="2">
         <v>0</v>
@@ -6536,7 +6537,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>65</v>
@@ -6605,13 +6606,13 @@
         <v>0</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB26" s="2">
         <v>1.2465753420000001</v>
       </c>
       <c r="AC26" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD26" s="2">
         <v>0</v>
@@ -6758,12 +6759,12 @@
         <v>40907</v>
       </c>
     </row>
-    <row r="27" spans="1:77" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:77" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
         <v>65</v>
@@ -6814,7 +6815,7 @@
         <v>2</v>
       </c>
       <c r="S27" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="U27">
         <v>2</v>
@@ -6835,13 +6836,13 @@
         <v>5</v>
       </c>
       <c r="AA27" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB27">
         <v>0</v>
       </c>
       <c r="AC27" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD27">
         <v>0</v>
@@ -6993,7 +6994,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
         <v>65</v>
@@ -7062,13 +7063,13 @@
         <v>0</v>
       </c>
       <c r="AA28" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB28">
         <v>0</v>
       </c>
       <c r="AC28" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD28">
         <v>0</v>
@@ -7220,7 +7221,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
         <v>65</v>
@@ -7289,13 +7290,13 @@
         <v>0</v>
       </c>
       <c r="AA29" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB29">
         <v>0</v>
       </c>
       <c r="AC29" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD29">
         <v>0.05</v>
@@ -7447,7 +7448,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
         <v>65</v>
@@ -7516,13 +7517,13 @@
         <v>0</v>
       </c>
       <c r="AA30" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB30">
         <v>0</v>
       </c>
       <c r="AC30" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD30">
         <v>0</v>
@@ -7674,7 +7675,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31" t="s">
         <v>65</v>
@@ -7743,13 +7744,13 @@
         <v>0</v>
       </c>
       <c r="AA31" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB31">
         <v>0</v>
       </c>
       <c r="AC31" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD31">
         <v>0</v>
@@ -7896,12 +7897,12 @@
         <v>40907</v>
       </c>
     </row>
-    <row r="32" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>41</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>65</v>
@@ -7952,7 +7953,7 @@
         <v>2</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="U32" s="2">
         <v>2</v>
@@ -7973,13 +7974,13 @@
         <v>4</v>
       </c>
       <c r="AA32" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB32" s="2">
         <v>0</v>
       </c>
       <c r="AC32" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AD32" s="2">
         <v>0</v>
@@ -8127,12 +8128,12 @@
         <v>40907</v>
       </c>
     </row>
-    <row r="33" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:77" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>42</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>65</v>
@@ -8183,7 +8184,7 @@
         <v>2</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="U33" s="2">
         <v>2</v>
@@ -8204,13 +8205,13 @@
         <v>4</v>
       </c>
       <c r="AA33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB33" s="2">
         <v>0</v>
       </c>
       <c r="AC33" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AD33" s="2">
         <v>0</v>

</xml_diff>